<commit_message>
getAllSeats function  now returns a list instead of an array
</commit_message>
<xml_diff>
--- a/analysis/Database/Book2.xlsx
+++ b/analysis/Database/Book2.xlsx
@@ -177,7 +177,40 @@
   <cols>
     <col min="4" max="4" width="13.71" style="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
getMySeats function now returns a list instead of array of string
</commit_message>
<xml_diff>
--- a/analysis/Database/Book2.xlsx
+++ b/analysis/Database/Book2.xlsx
@@ -180,7 +180,7 @@
   <sheetData>
     <row r="1">
       <c r="A1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -188,7 +188,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -196,7 +196,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -204,9 +204,41 @@
     </row>
     <row r="4">
       <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>